<commit_message>
remove drawGraphNode in examples
</commit_message>
<xml_diff>
--- a/Examples/AHP_Ratings_Cars/carModel_Ratings_Criteria_initialresults.xlsx
+++ b/Examples/AHP_Ratings_Cars/carModel_Ratings_Criteria_initialresults.xlsx
@@ -16,6 +16,8 @@
     <sheet name="Graph Model1" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Graph Model2" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Graph Model3" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Graph Model4" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Graph Model5" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,6 +439,72 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="13144500" cy="2790825"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="13144500" cy="2790825"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1103,6 +1171,20 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="9">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="11">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H14">
     <cfRule type="dataBar" priority="1">
@@ -1133,8 +1215,60 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="9">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="11">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>